<commit_message>
Google Colab stand alone notebook
</commit_message>
<xml_diff>
--- a/tutorials/data/JustAnExample.xlsx
+++ b/tutorials/data/JustAnExample.xlsx
@@ -225,7 +225,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="240">
   <si>
     <t>THICKNESS</t>
   </si>
@@ -897,9 +897,6 @@
   </si>
   <si>
     <t>sh</t>
-  </si>
-  <si>
-    <t>bs</t>
   </si>
   <si>
     <t>THESE LITHOLOGIES CAN'T BE EXPORTED TO SEDLOG  BECAUSE SEDLOG DOESN'T HAVE THESE</t>
@@ -1547,8 +1544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1637,7 +1634,7 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D3">
         <v>30</v>
@@ -1660,16 +1657,16 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J4" t="s">
         <v>40</v>
@@ -1677,7 +1674,7 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D5">
         <v>20</v>
@@ -1695,7 +1692,7 @@
         <v>36</v>
       </c>
       <c r="J5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K5" t="s">
         <v>71</v>
@@ -1703,16 +1700,16 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D6">
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J6" t="s">
         <v>151</v>
@@ -1720,7 +1717,7 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D7">
         <v>20</v>
@@ -1738,7 +1735,7 @@
         <v>9</v>
       </c>
       <c r="J7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K7" t="s">
         <v>72</v>
@@ -1746,16 +1743,16 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D8">
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J8" t="s">
         <v>40</v>
@@ -1763,7 +1760,7 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D9">
         <v>30</v>
@@ -1781,15 +1778,15 @@
         <v>9</v>
       </c>
       <c r="J9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D10">
         <v>23</v>
@@ -1807,21 +1804,21 @@
         <v>9</v>
       </c>
       <c r="J10" t="s">
+        <v>236</v>
+      </c>
+      <c r="K10" t="s">
         <v>237</v>
-      </c>
-      <c r="K10" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D11">
         <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H11" t="s">
         <v>15</v>
@@ -1829,7 +1826,7 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D12">
         <v>10</v>
@@ -1852,13 +1849,13 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D13">
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>16</v>
+        <v>217</v>
       </c>
       <c r="H13" t="s">
         <v>14</v>
@@ -1866,7 +1863,7 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D14">
         <v>30</v>
@@ -1880,13 +1877,13 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D15">
         <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="H15" t="s">
         <v>9</v>
@@ -1915,7 +1912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:O40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
@@ -2724,7 +2721,7 @@
     </row>
     <row r="40" spans="2:3" ht="60">
       <c r="C40" s="17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>